<commit_message>
relation and indexing problem v1.1
</commit_message>
<xml_diff>
--- a/dbs/doc/DB Architecture.xlsx
+++ b/dbs/doc/DB Architecture.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ExampleJohn\Desktop\8semestr\PAI gr1\projekt końcowy\git\dbs\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37F5E89D-5F09-42DC-AF98-1A24CCF5A46B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35E6EE44-F1E3-4888-8DE5-FD831784166D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23070" windowHeight="13500" xr2:uid="{E59D0004-C185-4289-B9BB-FE154D505BF8}"/>
   </bookViews>
@@ -41,9 +41,6 @@
     <t>User_ID (PK)</t>
   </si>
   <si>
-    <t>BIGSERIES</t>
-  </si>
-  <si>
     <t>VARCHAR 255</t>
   </si>
   <si>
@@ -264,6 +261,9 @@
   </si>
   <si>
     <t>Project</t>
+  </si>
+  <si>
+    <t>BIGINT 20</t>
   </si>
 </sst>
 </file>
@@ -373,15 +373,6 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -391,7 +382,16 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -710,8 +710,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ECAD0B67-0D9E-43E2-9E49-3D042561B2CF}">
   <dimension ref="A1:N54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="F26" sqref="F26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -730,39 +730,39 @@
         <v>0</v>
       </c>
       <c r="B1" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="C1" t="s">
         <v>29</v>
-      </c>
-      <c r="C1" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B2" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="C2" t="s">
         <v>35</v>
-      </c>
-      <c r="C2" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A4" s="18" t="s">
-        <v>39</v>
-      </c>
-      <c r="B4" s="18"/>
+      <c r="A4" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="B4" s="15"/>
       <c r="J4" s="9"/>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
@@ -770,47 +770,47 @@
         <v>1</v>
       </c>
       <c r="B5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>76</v>
+      </c>
+      <c r="B6" t="s">
         <v>2</v>
       </c>
-      <c r="B6" t="s">
-        <v>3</v>
-      </c>
       <c r="C6" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D6" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E6" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="J6" s="10"/>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A8" s="19" t="s">
-        <v>9</v>
-      </c>
-      <c r="B8" s="19"/>
+      <c r="A8" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="16"/>
       <c r="F8" s="8"/>
       <c r="G8" s="8"/>
       <c r="H8" s="8"/>
@@ -823,13 +823,13 @@
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" t="s">
+        <v>4</v>
+      </c>
+      <c r="C9" t="s">
         <v>11</v>
-      </c>
-      <c r="B9" t="s">
-        <v>5</v>
-      </c>
-      <c r="C9" t="s">
-        <v>12</v>
       </c>
       <c r="F9" s="8"/>
       <c r="G9" s="8"/>
@@ -843,449 +843,449 @@
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>76</v>
+      </c>
+      <c r="B10" t="s">
         <v>2</v>
       </c>
-      <c r="B10" t="s">
-        <v>3</v>
-      </c>
       <c r="C10" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A12" s="15" t="s">
-        <v>14</v>
-      </c>
-      <c r="B12" s="15"/>
-      <c r="C12" s="15"/>
+      <c r="A12" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12" s="17"/>
+      <c r="C12" s="17"/>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13" t="s">
         <v>15</v>
       </c>
-      <c r="B13" t="s">
-        <v>16</v>
-      </c>
       <c r="C13" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>2</v>
+        <v>76</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A16" s="20" t="s">
-        <v>19</v>
-      </c>
-      <c r="B16" s="20"/>
+      <c r="A16" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="B16" s="18"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
+        <v>19</v>
+      </c>
+      <c r="B17" t="s">
+        <v>12</v>
+      </c>
+      <c r="C17" t="s">
         <v>20</v>
       </c>
-      <c r="B17" t="s">
-        <v>13</v>
-      </c>
-      <c r="C17" t="s">
+      <c r="D17" t="s">
+        <v>71</v>
+      </c>
+      <c r="E17" t="s">
         <v>21</v>
       </c>
-      <c r="D17" t="s">
-        <v>72</v>
-      </c>
-      <c r="E17" t="s">
-        <v>22</v>
-      </c>
       <c r="F17" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
+        <v>76</v>
+      </c>
+      <c r="B18" t="s">
         <v>2</v>
       </c>
-      <c r="B18" t="s">
-        <v>3</v>
-      </c>
       <c r="C18" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D18" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E18" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F18" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="15" t="s">
-        <v>25</v>
-      </c>
-      <c r="B20" s="15"/>
-      <c r="C20" s="15"/>
+      <c r="A20" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="B20" s="17"/>
+      <c r="C20" s="17"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
+        <v>14</v>
+      </c>
+      <c r="B21" t="s">
+        <v>25</v>
+      </c>
+      <c r="C21" t="s">
         <v>15</v>
-      </c>
-      <c r="B21" t="s">
-        <v>26</v>
-      </c>
-      <c r="C21" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>2</v>
+        <v>76</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="17" t="s">
-        <v>38</v>
-      </c>
-      <c r="B24" s="17"/>
+      <c r="A24" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="B24" s="14"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B25" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C25" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D25" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E25" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F25" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G25" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
+        <v>76</v>
+      </c>
+      <c r="B26" t="s">
         <v>2</v>
       </c>
-      <c r="B26" t="s">
-        <v>3</v>
-      </c>
       <c r="C26" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E26" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F26" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G26" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" s="15" t="s">
-        <v>41</v>
-      </c>
-      <c r="B28" s="15"/>
-      <c r="C28" s="15"/>
+      <c r="A28" s="17" t="s">
+        <v>40</v>
+      </c>
+      <c r="B28" s="17"/>
+      <c r="C28" s="17"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
+        <v>14</v>
+      </c>
+      <c r="B29" t="s">
+        <v>32</v>
+      </c>
+      <c r="C29" t="s">
         <v>15</v>
-      </c>
-      <c r="B29" t="s">
-        <v>33</v>
-      </c>
-      <c r="C29" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>2</v>
+        <v>76</v>
       </c>
       <c r="B30" s="11" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A32" s="14" t="s">
-        <v>37</v>
-      </c>
-      <c r="B32" s="14"/>
+      <c r="A32" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="B32" s="19"/>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B33" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C33" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D33" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E33" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F33" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
+        <v>76</v>
+      </c>
+      <c r="B34" t="s">
         <v>2</v>
       </c>
-      <c r="B34" t="s">
-        <v>3</v>
-      </c>
       <c r="C34" s="11" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E34" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F34" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A36" s="15" t="s">
-        <v>44</v>
-      </c>
-      <c r="B36" s="15"/>
-      <c r="C36" s="15"/>
+      <c r="A36" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="B36" s="17"/>
+      <c r="C36" s="17"/>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
+        <v>14</v>
+      </c>
+      <c r="B37" t="s">
+        <v>44</v>
+      </c>
+      <c r="C37" t="s">
         <v>15</v>
-      </c>
-      <c r="B37" t="s">
-        <v>45</v>
-      </c>
-      <c r="C37" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>2</v>
+        <v>76</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A40" s="16" t="s">
-        <v>42</v>
-      </c>
-      <c r="B40" s="16"/>
+      <c r="A40" s="20" t="s">
+        <v>41</v>
+      </c>
+      <c r="B40" s="20"/>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B41" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C41" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D41" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E41" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>2</v>
+        <v>76</v>
       </c>
       <c r="B42" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D42" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E42" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" s="13" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B44" s="13"/>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B45" t="s">
+        <v>51</v>
+      </c>
+      <c r="C45" t="s">
+        <v>65</v>
+      </c>
+      <c r="D45" t="s">
+        <v>17</v>
+      </c>
+      <c r="E45" t="s">
         <v>52</v>
       </c>
-      <c r="C45" t="s">
-        <v>66</v>
-      </c>
-      <c r="D45" t="s">
-        <v>18</v>
-      </c>
-      <c r="E45" t="s">
-        <v>53</v>
-      </c>
       <c r="F45" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="G45" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>2</v>
+        <v>76</v>
       </c>
       <c r="B46" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C46" s="12" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D46" s="6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E46" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F46" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G46" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B48" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C48" t="s">
+        <v>55</v>
+      </c>
+      <c r="D48" t="s">
         <v>56</v>
       </c>
-      <c r="D48" t="s">
+      <c r="E48" t="s">
         <v>57</v>
       </c>
-      <c r="E48" t="s">
-        <v>58</v>
-      </c>
       <c r="F48" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
+        <v>60</v>
+      </c>
+      <c r="B49" t="s">
+        <v>5</v>
+      </c>
+      <c r="C49" t="s">
+        <v>5</v>
+      </c>
+      <c r="D49" t="s">
+        <v>22</v>
+      </c>
+      <c r="E49" t="s">
+        <v>22</v>
+      </c>
+      <c r="F49" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A52" s="17" t="s">
         <v>61</v>
       </c>
-      <c r="B49" t="s">
-        <v>6</v>
-      </c>
-      <c r="C49" t="s">
-        <v>6</v>
-      </c>
-      <c r="D49" t="s">
-        <v>23</v>
-      </c>
-      <c r="E49" t="s">
-        <v>23</v>
-      </c>
-      <c r="F49" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A52" s="15" t="s">
-        <v>62</v>
-      </c>
-      <c r="B52" s="15"/>
-      <c r="C52" s="15"/>
+      <c r="B52" s="17"/>
+      <c r="C52" s="17"/>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
+        <v>14</v>
+      </c>
+      <c r="B53" t="s">
+        <v>62</v>
+      </c>
+      <c r="C53" t="s">
         <v>15</v>
-      </c>
-      <c r="B53" t="s">
-        <v>63</v>
-      </c>
-      <c r="C53" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>2</v>
+        <v>76</v>
       </c>
       <c r="B54" s="13" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="A32:B32"/>
+    <mergeCell ref="A28:C28"/>
+    <mergeCell ref="A36:C36"/>
+    <mergeCell ref="A40:B40"/>
+    <mergeCell ref="A52:C52"/>
     <mergeCell ref="A24:B24"/>
     <mergeCell ref="A4:B4"/>
     <mergeCell ref="A8:B8"/>
     <mergeCell ref="A12:C12"/>
     <mergeCell ref="A16:B16"/>
     <mergeCell ref="A20:C20"/>
-    <mergeCell ref="A32:B32"/>
-    <mergeCell ref="A28:C28"/>
-    <mergeCell ref="A36:C36"/>
-    <mergeCell ref="A40:B40"/>
-    <mergeCell ref="A52:C52"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
indexing and relations v1.1
</commit_message>
<xml_diff>
--- a/dbs/doc/DB Architecture.xlsx
+++ b/dbs/doc/DB Architecture.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ExampleJohn\Desktop\8semestr\PAI gr1\projekt końcowy\git\dbs\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35E6EE44-F1E3-4888-8DE5-FD831784166D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96A46185-A8FC-4A13-9DC0-E5D981593561}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23070" windowHeight="13500" xr2:uid="{E59D0004-C185-4289-B9BB-FE154D505BF8}"/>
   </bookViews>
@@ -251,9 +251,6 @@
     <t>Description (N)</t>
   </si>
   <si>
-    <t>VARCHAR 5</t>
-  </si>
-  <si>
     <t>VARCHAR 4</t>
   </si>
   <si>
@@ -263,7 +260,10 @@
     <t>Project</t>
   </si>
   <si>
-    <t>BIGINT 20</t>
+    <t>INT 11</t>
+  </si>
+  <si>
+    <t>VARCHAR 6</t>
   </si>
 </sst>
 </file>
@@ -373,6 +373,15 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -382,16 +391,7 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -711,7 +711,7 @@
   <dimension ref="A1:N54"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="L6" sqref="L6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -759,10 +759,10 @@
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A4" s="15" t="s">
+      <c r="A4" s="18" t="s">
         <v>38</v>
       </c>
-      <c r="B4" s="15"/>
+      <c r="B4" s="18"/>
       <c r="J4" s="9"/>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
@@ -787,7 +787,7 @@
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B6" t="s">
         <v>2</v>
@@ -796,7 +796,7 @@
         <v>2</v>
       </c>
       <c r="D6" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="E6" t="s">
         <v>2</v>
@@ -807,10 +807,10 @@
       <c r="J6" s="10"/>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A8" s="16" t="s">
+      <c r="A8" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="16"/>
+      <c r="B8" s="19"/>
       <c r="F8" s="8"/>
       <c r="G8" s="8"/>
       <c r="H8" s="8"/>
@@ -843,21 +843,21 @@
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B10" t="s">
         <v>2</v>
       </c>
       <c r="C10" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A12" s="17" t="s">
+      <c r="A12" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="B12" s="17"/>
-      <c r="C12" s="17"/>
+      <c r="B12" s="15"/>
+      <c r="C12" s="15"/>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
@@ -872,7 +872,7 @@
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>16</v>
@@ -882,10 +882,10 @@
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A16" s="18" t="s">
+      <c r="A16" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="B16" s="18"/>
+      <c r="B16" s="20"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
@@ -909,7 +909,7 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B18" t="s">
         <v>2</v>
@@ -928,11 +928,11 @@
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="17" t="s">
+      <c r="A20" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="B20" s="17"/>
-      <c r="C20" s="17"/>
+      <c r="B20" s="15"/>
+      <c r="C20" s="15"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
@@ -947,7 +947,7 @@
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B22" s="5" t="s">
         <v>26</v>
@@ -957,10 +957,10 @@
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="14" t="s">
+      <c r="A24" s="17" t="s">
         <v>37</v>
       </c>
-      <c r="B24" s="14"/>
+      <c r="B24" s="17"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
@@ -970,7 +970,7 @@
         <v>12</v>
       </c>
       <c r="C25" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D25" t="s">
         <v>67</v>
@@ -987,7 +987,7 @@
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B26" t="s">
         <v>2</v>
@@ -1009,11 +1009,11 @@
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" s="17" t="s">
+      <c r="A28" s="15" t="s">
         <v>40</v>
       </c>
-      <c r="B28" s="17"/>
-      <c r="C28" s="17"/>
+      <c r="B28" s="15"/>
+      <c r="C28" s="15"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
@@ -1028,7 +1028,7 @@
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B30" s="11" t="s">
         <v>33</v>
@@ -1038,10 +1038,10 @@
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A32" s="19" t="s">
+      <c r="A32" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="B32" s="19"/>
+      <c r="B32" s="14"/>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
@@ -1051,7 +1051,7 @@
         <v>4</v>
       </c>
       <c r="C33" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D33" t="s">
         <v>66</v>
@@ -1065,7 +1065,7 @@
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B34" t="s">
         <v>2</v>
@@ -1084,11 +1084,11 @@
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A36" s="17" t="s">
+      <c r="A36" s="15" t="s">
         <v>43</v>
       </c>
-      <c r="B36" s="17"/>
-      <c r="C36" s="17"/>
+      <c r="B36" s="15"/>
+      <c r="C36" s="15"/>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
@@ -1103,7 +1103,7 @@
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B38" s="1" t="s">
         <v>45</v>
@@ -1113,10 +1113,10 @@
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A40" s="20" t="s">
+      <c r="A40" s="16" t="s">
         <v>41</v>
       </c>
-      <c r="B40" s="20"/>
+      <c r="B40" s="16"/>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
@@ -1137,7 +1137,7 @@
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B42" t="s">
         <v>47</v>
@@ -1183,7 +1183,7 @@
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B46" t="s">
         <v>47</v>
@@ -1245,11 +1245,11 @@
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A52" s="17" t="s">
+      <c r="A52" s="15" t="s">
         <v>61</v>
       </c>
-      <c r="B52" s="17"/>
-      <c r="C52" s="17"/>
+      <c r="B52" s="15"/>
+      <c r="C52" s="15"/>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
@@ -1264,7 +1264,7 @@
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B54" s="13" t="s">
         <v>50</v>
@@ -1275,17 +1275,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="A32:B32"/>
-    <mergeCell ref="A28:C28"/>
-    <mergeCell ref="A36:C36"/>
-    <mergeCell ref="A40:B40"/>
-    <mergeCell ref="A52:C52"/>
     <mergeCell ref="A24:B24"/>
     <mergeCell ref="A4:B4"/>
     <mergeCell ref="A8:B8"/>
     <mergeCell ref="A12:C12"/>
     <mergeCell ref="A16:B16"/>
     <mergeCell ref="A20:C20"/>
+    <mergeCell ref="A32:B32"/>
+    <mergeCell ref="A28:C28"/>
+    <mergeCell ref="A36:C36"/>
+    <mergeCell ref="A40:B40"/>
+    <mergeCell ref="A52:C52"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
BD Arch with relations and siple data insertions
</commit_message>
<xml_diff>
--- a/dbs/doc/DB Architecture.xlsx
+++ b/dbs/doc/DB Architecture.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ExampleJohn\Desktop\8semestr\PAI gr1\projekt końcowy\git\dbs\doc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\EXAMPLEJOHN-PC\Users\ExampleJohn\Desktop\8semestr\PAI gr1\projekt końcowy\git\dbs\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96A46185-A8FC-4A13-9DC0-E5D981593561}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{531AB1EB-97D9-478B-A898-D385139E00AA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23070" windowHeight="13500" xr2:uid="{E59D0004-C185-4289-B9BB-FE154D505BF8}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="19800" windowHeight="11760" xr2:uid="{E59D0004-C185-4289-B9BB-FE154D505BF8}"/>
   </bookViews>
   <sheets>
     <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="75">
   <si>
     <t>Nazwa</t>
   </si>
@@ -227,18 +227,6 @@
     <t>Position</t>
   </si>
   <si>
-    <t>Int</t>
-  </si>
-  <si>
-    <t>Column (U)</t>
-  </si>
-  <si>
-    <t>C_Leader</t>
-  </si>
-  <si>
-    <t>P_Leader</t>
-  </si>
-  <si>
     <t>Null</t>
   </si>
   <si>
@@ -254,16 +242,22 @@
     <t>VARCHAR 4</t>
   </si>
   <si>
-    <t>Organisation</t>
-  </si>
-  <si>
-    <t>Project</t>
-  </si>
-  <si>
     <t>INT 11</t>
   </si>
   <si>
     <t>VARCHAR 6</t>
+  </si>
+  <si>
+    <t>Proj_Leader_ID</t>
+  </si>
+  <si>
+    <t>Project_ID</t>
+  </si>
+  <si>
+    <t>Chart_Leader</t>
+  </si>
+  <si>
+    <t>INT 2</t>
   </si>
 </sst>
 </file>
@@ -710,8 +704,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ECAD0B67-0D9E-43E2-9E49-3D042561B2CF}">
   <dimension ref="A1:N54"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L6" sqref="L6"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="E43" sqref="E43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -719,7 +713,8 @@
     <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9.5703125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="14.5703125" bestFit="1" customWidth="1"/>
     <col min="8" max="9" width="9.5703125" bestFit="1" customWidth="1"/>
@@ -752,10 +747,10 @@
         <v>7</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="C3" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
@@ -779,7 +774,7 @@
         <v>11</v>
       </c>
       <c r="E5" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="F5" t="s">
         <v>23</v>
@@ -787,7 +782,7 @@
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="B6" t="s">
         <v>2</v>
@@ -796,7 +791,7 @@
         <v>2</v>
       </c>
       <c r="D6" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="E6" t="s">
         <v>2</v>
@@ -843,13 +838,13 @@
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="B10" t="s">
         <v>2</v>
       </c>
       <c r="C10" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
@@ -872,7 +867,7 @@
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>16</v>
@@ -898,7 +893,7 @@
         <v>20</v>
       </c>
       <c r="D17" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="E17" t="s">
         <v>21</v>
@@ -909,7 +904,7 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="B18" t="s">
         <v>2</v>
@@ -947,7 +942,7 @@
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="B22" s="5" t="s">
         <v>26</v>
@@ -970,13 +965,13 @@
         <v>12</v>
       </c>
       <c r="C25" t="s">
-        <v>73</v>
+        <v>26</v>
       </c>
       <c r="D25" t="s">
+        <v>71</v>
+      </c>
+      <c r="E25" t="s">
         <v>67</v>
-      </c>
-      <c r="E25" t="s">
-        <v>71</v>
       </c>
       <c r="F25" t="s">
         <v>21</v>
@@ -987,7 +982,7 @@
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="B26" t="s">
         <v>2</v>
@@ -1028,7 +1023,7 @@
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="B30" s="11" t="s">
         <v>33</v>
@@ -1051,13 +1046,13 @@
         <v>4</v>
       </c>
       <c r="C33" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D33" t="s">
-        <v>66</v>
+        <v>73</v>
       </c>
       <c r="E33" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="F33" t="s">
         <v>21</v>
@@ -1065,7 +1060,7 @@
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="B34" t="s">
         <v>2</v>
@@ -1103,7 +1098,7 @@
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="B38" s="1" t="s">
         <v>45</v>
@@ -1126,7 +1121,7 @@
         <v>4</v>
       </c>
       <c r="C41" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D41" t="s">
         <v>48</v>
@@ -1137,7 +1132,7 @@
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="B42" t="s">
         <v>47</v>
@@ -1149,7 +1144,7 @@
         <v>22</v>
       </c>
       <c r="E42" t="s">
-        <v>64</v>
+        <v>74</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
@@ -1166,7 +1161,7 @@
         <v>51</v>
       </c>
       <c r="C45" t="s">
-        <v>65</v>
+        <v>46</v>
       </c>
       <c r="D45" t="s">
         <v>17</v>
@@ -1178,12 +1173,12 @@
         <v>59</v>
       </c>
       <c r="G45" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="B46" t="s">
         <v>47</v>
@@ -1264,7 +1259,7 @@
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="B54" s="13" t="s">
         <v>50</v>

</xml_diff>